<commit_message>
some changes to the paper, metal, organic, glass classes
moved some data from metal to glass, deleted entries from metal, organic, and paper
</commit_message>
<xml_diff>
--- a/ensc424_waste_classification_testcases.xlsx
+++ b/ensc424_waste_classification_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansle\ensc424-waste-classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07281C5F-1F1B-43E0-810C-EE8AC6139BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829AC98D-C831-4745-A555-4AAE5C516D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{FBB36D13-CA9D-4E47-8343-E7942F3BEC57}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{FBB36D13-CA9D-4E47-8343-E7942F3BEC57}"/>
   </bookViews>
   <sheets>
     <sheet name="AlexNet" sheetId="1" r:id="rId1"/>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6878BB8-0EAE-4C46-8D5C-AA38530424C8}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="A1:M3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF612EF1-B939-4BF9-AFCF-8B702F8358AD}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,15 +640,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F416109C0AA5244181E3F8ADB71ABB3E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7aa50a603bcf0d946c6ee69eec6587de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="da2ea8e4-410b-4722-8052-f32ecc8b34ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb983a1bcd3bd0b77289e13891ab6baa" ns3:_="">
     <xsd:import namespace="da2ea8e4-410b-4722-8052-f32ecc8b34ac"/>
@@ -780,6 +771,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -787,14 +787,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{243D645E-FF63-4971-98EC-64FDC8EAF9D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42C4E1A9-1662-4FB0-95B5-3F7EE514700A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -812,6 +804,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{243D645E-FF63-4971-98EC-64FDC8EAF9D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D6AED09-99DE-442D-9592-AD20244AF1E9}">
   <ds:schemaRefs>

</xml_diff>